<commit_message>
huge changes on every front
</commit_message>
<xml_diff>
--- a/admin/data/templates/themenliste.xlsx
+++ b/admin/data/templates/themenliste.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="154">
   <si>
     <t>Titel der Stunde</t>
   </si>
@@ -56,19 +56,31 @@
     <t>Mi</t>
   </si>
   <si>
+    <t>Die Reihenfolge der Spalten darf nicht verändert werden!</t>
+  </si>
+  <si>
     <t>Therme aufstellen, mit einer Unbekannten lösen</t>
   </si>
   <si>
     <t>Do</t>
   </si>
   <si>
+    <t>Keine leeren Zeilen hinzufügen!</t>
+  </si>
+  <si>
     <t>Dreisatz, Übungen</t>
   </si>
   <si>
     <t>Fr</t>
   </si>
   <si>
+    <t>Die Tabelle kann nach unten hin erweitert werden, wenn ein neues Fach dazukommt.</t>
+  </si>
+  <si>
     <t>Prozent- und Zinsrechnung</t>
+  </si>
+  <si>
+    <t>Farbcodierungen oder ähnliches sind kein Problem.</t>
   </si>
   <si>
     <t>Lineare Zuordnungen im Koordinatensystem</t>
@@ -474,7 +486,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -502,6 +514,19 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF800000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF800000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -552,12 +577,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -639,10 +672,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F151"/>
+  <dimension ref="A1:H151"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -653,7 +686,9 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.33163265306122"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4744897959184"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.9897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -735,10 +770,13 @@
       <c r="F4" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>7</v>
@@ -747,18 +785,21 @@
         <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>7</v>
@@ -767,18 +808,21 @@
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>7</v>
@@ -794,11 +838,14 @@
       </c>
       <c r="F7" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>7</v>
@@ -818,7 +865,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>7</v>
@@ -838,7 +885,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>7</v>
@@ -847,7 +894,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>3</v>
@@ -858,7 +905,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>7</v>
@@ -867,7 +914,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>3</v>
@@ -878,7 +925,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>7</v>
@@ -898,7 +945,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>7</v>
@@ -918,7 +965,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>7</v>
@@ -938,7 +985,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>7</v>
@@ -947,7 +994,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>2</v>
@@ -958,7 +1005,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>7</v>
@@ -967,7 +1014,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>2</v>
@@ -978,7 +1025,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>7</v>
@@ -998,7 +1045,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>7</v>
@@ -1018,7 +1065,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>7</v>
@@ -1038,7 +1085,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>7</v>
@@ -1047,7 +1094,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>1</v>
@@ -1058,7 +1105,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>7</v>
@@ -1067,7 +1114,7 @@
         <v>9</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>1</v>
@@ -1078,7 +1125,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>7</v>
@@ -1098,7 +1145,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>7</v>
@@ -1118,7 +1165,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>7</v>
@@ -1138,7 +1185,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>7</v>
@@ -1147,7 +1194,7 @@
         <v>10</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>3</v>
@@ -1158,7 +1205,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>7</v>
@@ -1167,7 +1214,7 @@
         <v>10</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>3</v>
@@ -1178,10 +1225,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>7</v>
@@ -1198,10 +1245,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>7</v>
@@ -1218,10 +1265,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>7</v>
@@ -1238,16 +1285,16 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>7</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>2</v>
@@ -1258,16 +1305,16 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="C31" s="0" t="n">
         <v>7</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>2</v>
@@ -1278,10 +1325,10 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>8</v>
@@ -1298,10 +1345,10 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>8</v>
@@ -1318,10 +1365,10 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>8</v>
@@ -1338,16 +1385,16 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>1</v>
@@ -1358,16 +1405,16 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>1</v>
@@ -1378,10 +1425,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>9</v>
@@ -1398,10 +1445,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>9</v>
@@ -1418,10 +1465,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>9</v>
@@ -1438,16 +1485,16 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>9</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>3</v>
@@ -1458,16 +1505,16 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>9</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>3</v>
@@ -1478,10 +1525,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>10</v>
@@ -1498,10 +1545,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>10</v>
@@ -1518,10 +1565,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>10</v>
@@ -1538,16 +1585,16 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>2</v>
@@ -1558,16 +1605,16 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>2</v>
@@ -1578,10 +1625,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>8</v>
@@ -1598,10 +1645,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>8</v>
@@ -1618,10 +1665,10 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>8</v>
@@ -1638,16 +1685,16 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>3</v>
@@ -1658,16 +1705,16 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="B51" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="C51" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>3</v>
@@ -1678,10 +1725,10 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>9</v>
@@ -1698,10 +1745,10 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C53" s="0" t="n">
         <v>9</v>
@@ -1718,10 +1765,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C54" s="0" t="n">
         <v>9</v>
@@ -1738,16 +1785,16 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>9</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E55" s="0" t="n">
         <v>2</v>
@@ -1758,16 +1805,16 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>9</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E56" s="0" t="n">
         <v>2</v>
@@ -1778,10 +1825,10 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C57" s="0" t="n">
         <v>10</v>
@@ -1798,10 +1845,10 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C58" s="0" t="n">
         <v>10</v>
@@ -1818,10 +1865,10 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C59" s="0" t="n">
         <v>10</v>
@@ -1838,16 +1885,16 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C60" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>1</v>
@@ -1858,16 +1905,16 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C61" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>1</v>
@@ -1878,10 +1925,10 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C62" s="0" t="n">
         <v>6</v>
@@ -1898,10 +1945,10 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C63" s="0" t="n">
         <v>6</v>
@@ -1918,10 +1965,10 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C64" s="0" t="n">
         <v>6</v>
@@ -1938,16 +1985,16 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C65" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E65" s="0" t="n">
         <v>3</v>
@@ -1958,16 +2005,16 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B66" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="B66" s="0" t="s">
-        <v>73</v>
       </c>
       <c r="C66" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>3</v>
@@ -1978,10 +2025,10 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C67" s="0" t="n">
         <v>7</v>
@@ -1998,10 +2045,10 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C68" s="0" t="n">
         <v>7</v>
@@ -2018,10 +2065,10 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C69" s="0" t="n">
         <v>7</v>
@@ -2038,16 +2085,16 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C70" s="0" t="n">
         <v>7</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E70" s="0" t="n">
         <v>2</v>
@@ -2058,16 +2105,16 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C71" s="0" t="n">
         <v>7</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E71" s="0" t="n">
         <v>2</v>
@@ -2078,10 +2125,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C72" s="0" t="n">
         <v>8</v>
@@ -2098,10 +2145,10 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C73" s="0" t="n">
         <v>8</v>
@@ -2118,10 +2165,10 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C74" s="0" t="n">
         <v>8</v>
@@ -2138,16 +2185,16 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C75" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E75" s="0" t="n">
         <v>1</v>
@@ -2158,16 +2205,16 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C76" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E76" s="0" t="n">
         <v>1</v>
@@ -2178,10 +2225,10 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C77" s="0" t="n">
         <v>9</v>
@@ -2198,10 +2245,10 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C78" s="0" t="n">
         <v>9</v>
@@ -2218,10 +2265,10 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C79" s="0" t="n">
         <v>9</v>
@@ -2238,16 +2285,16 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C80" s="0" t="n">
         <v>9</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E80" s="0" t="n">
         <v>3</v>
@@ -2258,16 +2305,16 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C81" s="0" t="n">
         <v>9</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E81" s="0" t="n">
         <v>3</v>
@@ -2278,10 +2325,10 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C82" s="0" t="n">
         <v>10</v>
@@ -2298,10 +2345,10 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C83" s="0" t="n">
         <v>10</v>
@@ -2318,10 +2365,10 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C84" s="0" t="n">
         <v>10</v>
@@ -2338,16 +2385,16 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C85" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E85" s="0" t="n">
         <v>2</v>
@@ -2358,16 +2405,16 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C86" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>2</v>
@@ -2378,10 +2425,10 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C87" s="0" t="n">
         <v>6</v>
@@ -2398,10 +2445,10 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C88" s="0" t="n">
         <v>6</v>
@@ -2418,10 +2465,10 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C89" s="0" t="n">
         <v>6</v>
@@ -2438,16 +2485,16 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C90" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E90" s="0" t="n">
         <v>2</v>
@@ -2458,16 +2505,16 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B91" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="B91" s="0" t="s">
-        <v>99</v>
       </c>
       <c r="C91" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E91" s="0" t="n">
         <v>2</v>
@@ -2478,10 +2525,10 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C92" s="0" t="n">
         <v>7</v>
@@ -2498,10 +2545,10 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C93" s="0" t="n">
         <v>7</v>
@@ -2518,10 +2565,10 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C94" s="0" t="n">
         <v>7</v>
@@ -2538,16 +2585,16 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C95" s="0" t="n">
         <v>7</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E95" s="0" t="n">
         <v>1</v>
@@ -2558,16 +2605,16 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C96" s="0" t="n">
         <v>7</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E96" s="0" t="n">
         <v>1</v>
@@ -2578,10 +2625,10 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C97" s="0" t="n">
         <v>8</v>
@@ -2598,10 +2645,10 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C98" s="0" t="n">
         <v>8</v>
@@ -2618,10 +2665,10 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C99" s="0" t="n">
         <v>8</v>
@@ -2638,16 +2685,16 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C100" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E100" s="0" t="n">
         <v>3</v>
@@ -2658,16 +2705,16 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C101" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E101" s="0" t="n">
         <v>3</v>
@@ -2678,10 +2725,10 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C102" s="0" t="n">
         <v>9</v>
@@ -2698,10 +2745,10 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C103" s="0" t="n">
         <v>9</v>
@@ -2718,10 +2765,10 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C104" s="0" t="n">
         <v>9</v>
@@ -2738,16 +2785,16 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C105" s="0" t="n">
         <v>9</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E105" s="0" t="n">
         <v>2</v>
@@ -2758,16 +2805,16 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C106" s="0" t="n">
         <v>9</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E106" s="0" t="n">
         <v>2</v>
@@ -2778,10 +2825,10 @@
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C107" s="0" t="n">
         <v>10</v>
@@ -2798,10 +2845,10 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C108" s="0" t="n">
         <v>10</v>
@@ -2818,10 +2865,10 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C109" s="0" t="n">
         <v>10</v>
@@ -2838,16 +2885,16 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C110" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E110" s="0" t="n">
         <v>1</v>
@@ -2858,16 +2905,16 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C111" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E111" s="0" t="n">
         <v>1</v>
@@ -2878,10 +2925,10 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C112" s="0" t="n">
         <v>6</v>
@@ -2898,10 +2945,10 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C113" s="0" t="n">
         <v>6</v>
@@ -2918,10 +2965,10 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C114" s="0" t="n">
         <v>6</v>
@@ -2938,16 +2985,16 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C115" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E115" s="0" t="n">
         <v>2</v>
@@ -2958,16 +3005,16 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B116" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="B116" s="0" t="s">
-        <v>124</v>
       </c>
       <c r="C116" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E116" s="0" t="n">
         <v>2</v>
@@ -2978,10 +3025,10 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C117" s="0" t="n">
         <v>7</v>
@@ -2998,10 +3045,10 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C118" s="0" t="n">
         <v>7</v>
@@ -3018,10 +3065,10 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C119" s="0" t="n">
         <v>7</v>
@@ -3038,16 +3085,16 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C120" s="0" t="n">
         <v>7</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E120" s="0" t="n">
         <v>1</v>
@@ -3058,16 +3105,16 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C121" s="0" t="n">
         <v>7</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E121" s="0" t="n">
         <v>1</v>
@@ -3078,10 +3125,10 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C122" s="0" t="n">
         <v>8</v>
@@ -3098,10 +3145,10 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C123" s="0" t="n">
         <v>8</v>
@@ -3118,10 +3165,10 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C124" s="0" t="n">
         <v>8</v>
@@ -3138,16 +3185,16 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C125" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E125" s="0" t="n">
         <v>2</v>
@@ -3158,16 +3205,16 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C126" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E126" s="0" t="n">
         <v>2</v>
@@ -3178,10 +3225,10 @@
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C127" s="0" t="n">
         <v>9</v>
@@ -3198,10 +3245,10 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C128" s="0" t="n">
         <v>9</v>
@@ -3218,10 +3265,10 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C129" s="0" t="n">
         <v>9</v>
@@ -3238,16 +3285,16 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C130" s="0" t="n">
         <v>9</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E130" s="0" t="n">
         <v>1</v>
@@ -3258,16 +3305,16 @@
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C131" s="0" t="n">
         <v>9</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E131" s="0" t="n">
         <v>1</v>
@@ -3278,10 +3325,10 @@
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C132" s="0" t="n">
         <v>10</v>
@@ -3298,10 +3345,10 @@
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C133" s="0" t="n">
         <v>10</v>
@@ -3318,10 +3365,10 @@
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C134" s="0" t="n">
         <v>10</v>
@@ -3338,16 +3385,16 @@
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C135" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D135" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E135" s="0" t="n">
         <v>3</v>
@@ -3358,16 +3405,16 @@
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C136" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D136" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E136" s="0" t="n">
         <v>3</v>
@@ -3378,10 +3425,10 @@
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C137" s="0" t="n">
         <v>8</v>
@@ -3398,10 +3445,10 @@
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C138" s="0" t="n">
         <v>8</v>
@@ -3418,10 +3465,10 @@
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C139" s="0" t="n">
         <v>8</v>
@@ -3438,16 +3485,16 @@
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C140" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D140" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E140" s="0" t="n">
         <v>1</v>
@@ -3458,16 +3505,16 @@
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C141" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D141" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E141" s="0" t="n">
         <v>1</v>
@@ -3478,10 +3525,10 @@
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C142" s="0" t="n">
         <v>9</v>
@@ -3498,10 +3545,10 @@
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C143" s="0" t="n">
         <v>9</v>
@@ -3518,10 +3565,10 @@
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C144" s="0" t="n">
         <v>9</v>
@@ -3538,16 +3585,16 @@
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C145" s="0" t="n">
         <v>9</v>
       </c>
       <c r="D145" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E145" s="0" t="n">
         <v>3</v>
@@ -3558,16 +3605,16 @@
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B146" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C146" s="0" t="n">
         <v>9</v>
       </c>
       <c r="D146" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E146" s="0" t="n">
         <v>3</v>
@@ -3578,10 +3625,10 @@
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C147" s="0" t="n">
         <v>10</v>
@@ -3598,10 +3645,10 @@
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C148" s="0" t="n">
         <v>10</v>
@@ -3618,10 +3665,10 @@
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C149" s="0" t="n">
         <v>10</v>
@@ -3638,16 +3685,16 @@
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C150" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D150" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E150" s="0" t="n">
         <v>2</v>
@@ -3658,16 +3705,16 @@
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C151" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D151" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E151" s="0" t="n">
         <v>2</v>

</xml_diff>